<commit_message>
working id reaader 17.0
</commit_message>
<xml_diff>
--- a/be_id_reader/static/files/res_partner.xlsx
+++ b/be_id_reader/static/files/res_partner.xlsx
@@ -1,64 +1,73 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocol\Documents\BandIT\odoo\id-reader\be_id_reader\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocol\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBF1AA-E6DB-4693-98C6-6551119AEC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CCF52-54B3-4781-B5F3-E6186F3E3EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3168" yWindow="588" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="res_partner" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
   <si>
     <t>Date of birth</t>
   </si>
   <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Is a Company</t>
+  </si>
+  <si>
+    <t>Job Position</t>
+  </si>
+  <si>
+    <t>National identification number</t>
+  </si>
+  <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>Related Company</t>
   </si>
   <si>
     <t>Salesperson</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>National identification number</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Jérôme Dewandre</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Watermael-Boitsfort</t>
-  </si>
-  <si>
-    <t>95041328785</t>
-  </si>
-  <si>
-    <t>Name</t>
+    <t>Jhon Doe</t>
+  </si>
+  <si>
+    <t>Bruxelles</t>
   </si>
 </sst>
 </file>
@@ -418,64 +427,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="30.6640625" customWidth="1"/>
+    <col min="1" max="13" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3">
+        <v>35889</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3">
-        <v>34802</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>78586315785</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>